<commit_message>
truven dw_staging QA codes written
Final counts not yet run - wait for re-run of Joe's scripts
</commit_message>
<xml_diff>
--- a/greenplum/datawarehouse/QA/qa-all-db-checks/truven/dw_staging/outputs/truven-claim-header-counting.xlsx
+++ b/greenplum/datawarehouse/QA/qa-all-db-checks/truven/dw_staging/outputs/truven-claim-header-counting.xlsx
@@ -6,18 +6,19 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="claim-header" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="distinct-claim-ids" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="distinct-enrolid-clmid-combos" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="258">
   <si>
     <t xml:space="preserve">Count of distinct claim IDs (msclmid) in data_warehouse and Truven schema on TACC server</t>
   </si>
   <si>
-    <t xml:space="preserve">Run time: 2023-01-06 15:34:19</t>
+    <t xml:space="preserve">Run time: 2023-01-10 15:48:19</t>
   </si>
   <si>
     <t xml:space="preserve">year</t>
@@ -161,16 +162,7 @@
     <t xml:space="preserve">18332457</t>
   </si>
   <si>
-    <t xml:space="preserve">7236327</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36487140</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3849715</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18333150</t>
+    <t xml:space="preserve">18332458</t>
   </si>
   <si>
     <t xml:space="preserve">6715071</t>
@@ -185,16 +177,16 @@
     <t xml:space="preserve">16274140</t>
   </si>
   <si>
-    <t xml:space="preserve">6724984</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37550070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2960170</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16276747</t>
+    <t xml:space="preserve">6715083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37535115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2959578</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16275643</t>
   </si>
   <si>
     <t xml:space="preserve">7498578</t>
@@ -209,16 +201,16 @@
     <t xml:space="preserve">12651407</t>
   </si>
   <si>
-    <t xml:space="preserve">7508331</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50229030</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1993365</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12652141</t>
+    <t xml:space="preserve">7498614</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50220108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1993135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12651429</t>
   </si>
   <si>
     <t xml:space="preserve">6912678</t>
@@ -233,16 +225,13 @@
     <t xml:space="preserve">13361806</t>
   </si>
   <si>
-    <t xml:space="preserve">6920009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43892681</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1966388</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13363141</t>
+    <t xml:space="preserve">6912682</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1966294</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13362344</t>
   </si>
   <si>
     <t xml:space="preserve">6885922</t>
@@ -257,16 +246,13 @@
     <t xml:space="preserve">17636947</t>
   </si>
   <si>
-    <t xml:space="preserve">6892886</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46332613</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3092110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17638717</t>
+    <t xml:space="preserve">6885963</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3091594</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17636955</t>
   </si>
   <si>
     <t xml:space="preserve">6502122</t>
@@ -281,16 +267,16 @@
     <t xml:space="preserve">16446556</t>
   </si>
   <si>
-    <t xml:space="preserve">6517441</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43596836</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3265479</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16447223</t>
+    <t xml:space="preserve">6512965</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43595978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3265064</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16446722</t>
   </si>
   <si>
     <t xml:space="preserve">Difference between Truven schema and data_warehouse (Truven - DW):</t>
@@ -350,76 +336,457 @@
     <t xml:space="preserve">35</t>
   </si>
   <si>
-    <t xml:space="preserve">10598</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12837</t>
-  </si>
-  <si>
-    <t xml:space="preserve">577</t>
-  </si>
-  <si>
-    <t xml:space="preserve">693</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9913</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14959</t>
-  </si>
-  <si>
-    <t xml:space="preserve">791</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2607</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9753</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8931</t>
-  </si>
-  <si>
-    <t xml:space="preserve">313</t>
-  </si>
-  <si>
-    <t xml:space="preserve">734</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7331</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5262</t>
-  </si>
-  <si>
-    <t xml:space="preserve">223</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1335</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6964</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7653</t>
-  </si>
-  <si>
-    <t xml:space="preserve">599</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1770</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15319</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1608</t>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">199</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1503</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">129</t>
+  </si>
+  <si>
+    <t xml:space="preserve">538</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10843</t>
+  </si>
+  <si>
+    <t xml:space="preserve">750</t>
+  </si>
+  <si>
+    <t xml:space="preserve">141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">166</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: The difference in claim id count in 2021 is because some claims have enrolids that exist in the s and o tables that do not map to any enrolid in the a or t tables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The reason that this discrepancy ONLY exists in 2021 is likely because for 2020 and earlier, Will created entries in dim_uth_member_id to accomodate them</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count of distinct enrolid-clmid combinations in data_warehouse and Truven schema on TACC server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dw_concat_ccaes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dw_concat_ccaeo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dw_concat_mdcrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dw_concat_mdcro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">truv_concat_ccaes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">truv_concat_ccaeo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">truv_concat_mdcrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">truv_concat_mdcro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22342712</t>
+  </si>
+  <si>
+    <t xml:space="preserve">465722230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10836749</t>
+  </si>
+  <si>
+    <t xml:space="preserve">106577282</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21969951</t>
+  </si>
+  <si>
+    <t xml:space="preserve">475900752</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10014213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99439829</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21970613</t>
+  </si>
+  <si>
+    <t xml:space="preserve">475937095</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10014407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99450731</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16810842</t>
+  </si>
+  <si>
+    <t xml:space="preserve">374412587</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8711620</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88049251</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16811236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">374452089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8711802</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88058517</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17912725</t>
+  </si>
+  <si>
+    <t xml:space="preserve">399837010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7964483</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79527961</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17913281</t>
+  </si>
+  <si>
+    <t xml:space="preserve">399893091</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7964806</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79544566</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11501570</t>
+  </si>
+  <si>
+    <t xml:space="preserve">254839460</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5183966</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49718067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11502326</t>
+  </si>
+  <si>
+    <t xml:space="preserve">254905460</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5184314</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49736787</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11598289</t>
+  </si>
+  <si>
+    <t xml:space="preserve">264225196</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4812832</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48879459</t>
+  </si>
+  <si>
+    <t xml:space="preserve">264225211</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48879464</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10576804</t>
+  </si>
+  <si>
+    <t xml:space="preserve">245406257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3447047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34108265</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10577391</t>
+  </si>
+  <si>
+    <t xml:space="preserve">245443738</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3447394</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34120574</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10975901</t>
+  </si>
+  <si>
+    <t xml:space="preserve">251298798</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2341981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26092815</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10976706</t>
+  </si>
+  <si>
+    <t xml:space="preserve">251365411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2342184</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26105481</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10099974</t>
+  </si>
+  <si>
+    <t xml:space="preserve">236737939</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2272240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25782652</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10100319</t>
+  </si>
+  <si>
+    <t xml:space="preserve">236770305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2272431</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25794549</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9461807</t>
+  </si>
+  <si>
+    <t xml:space="preserve">216043806</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3361346</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31573004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9462462</t>
+  </si>
+  <si>
+    <t xml:space="preserve">216097356</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3361488</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31580107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9078284</t>
+  </si>
+  <si>
+    <t xml:space="preserve">226637768</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3571144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34268858</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9098129</t>
+  </si>
+  <si>
+    <t xml:space="preserve">226696842</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3571308</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34270777</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ccaes_concat_diff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ccaeo_concat_diff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mdcrs_concat_diff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mdcro_concat_diff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">662</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36343</t>
+  </si>
+  <si>
+    <t xml:space="preserve">194</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10902</t>
+  </si>
+  <si>
+    <t xml:space="preserve">394</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39502</t>
+  </si>
+  <si>
+    <t xml:space="preserve">182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9266</t>
   </si>
   <si>
     <t xml:space="preserve">556</t>
   </si>
   <si>
-    <t xml:space="preserve">667</t>
+    <t xml:space="preserve">56081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16605</t>
+  </si>
+  <si>
+    <t xml:space="preserve">756</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">348</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18720</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">587</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37481</t>
+  </si>
+  <si>
+    <t xml:space="preserve">347</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12309</t>
+  </si>
+  <si>
+    <t xml:space="preserve">805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66613</t>
+  </si>
+  <si>
+    <t xml:space="preserve">203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32366</t>
+  </si>
+  <si>
+    <t xml:space="preserve">191</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11897</t>
+  </si>
+  <si>
+    <t xml:space="preserve">655</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53550</t>
+  </si>
+  <si>
+    <t xml:space="preserve">142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19845</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59074</t>
+  </si>
+  <si>
+    <t xml:space="preserve">164</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1919</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: The difference in enrolid || claim id count in 2021 is because some claims have enrolids that exist in the s and o tables that do not map to any enrolid in the a or t tables</t>
   </si>
 </sst>
 </file>
@@ -964,16 +1331,16 @@
         <v>48</v>
       </c>
       <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" t="s">
         <v>49</v>
-      </c>
-      <c r="G10" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" t="s">
-        <v>51</v>
-      </c>
-      <c r="I10" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="11">
@@ -981,28 +1348,28 @@
         <v>2017</v>
       </c>
       <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" t="s">
         <v>53</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F11" t="s">
         <v>54</v>
       </c>
-      <c r="D11" t="s">
+      <c r="G11" t="s">
         <v>55</v>
       </c>
-      <c r="E11" t="s">
+      <c r="H11" t="s">
         <v>56</v>
       </c>
-      <c r="F11" t="s">
+      <c r="I11" t="s">
         <v>57</v>
-      </c>
-      <c r="G11" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" t="s">
-        <v>59</v>
-      </c>
-      <c r="I11" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="12">
@@ -1010,28 +1377,28 @@
         <v>2018</v>
       </c>
       <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" t="s">
         <v>61</v>
       </c>
-      <c r="C12" t="s">
+      <c r="F12" t="s">
         <v>62</v>
       </c>
-      <c r="D12" t="s">
+      <c r="G12" t="s">
         <v>63</v>
       </c>
-      <c r="E12" t="s">
+      <c r="H12" t="s">
         <v>64</v>
       </c>
-      <c r="F12" t="s">
+      <c r="I12" t="s">
         <v>65</v>
-      </c>
-      <c r="G12" t="s">
-        <v>66</v>
-      </c>
-      <c r="H12" t="s">
-        <v>67</v>
-      </c>
-      <c r="I12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="13">
@@ -1039,28 +1406,28 @@
         <v>2019</v>
       </c>
       <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" t="s">
         <v>69</v>
       </c>
-      <c r="C13" t="s">
+      <c r="F13" t="s">
         <v>70</v>
       </c>
-      <c r="D13" t="s">
+      <c r="G13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" t="s">
         <v>71</v>
       </c>
-      <c r="E13" t="s">
+      <c r="I13" t="s">
         <v>72</v>
-      </c>
-      <c r="F13" t="s">
-        <v>73</v>
-      </c>
-      <c r="G13" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" t="s">
-        <v>75</v>
-      </c>
-      <c r="I13" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="14">
@@ -1068,28 +1435,28 @@
         <v>2020</v>
       </c>
       <c r="B14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" t="s">
         <v>77</v>
       </c>
-      <c r="C14" t="s">
+      <c r="G14" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" t="s">
         <v>78</v>
       </c>
-      <c r="D14" t="s">
+      <c r="I14" t="s">
         <v>79</v>
-      </c>
-      <c r="E14" t="s">
-        <v>80</v>
-      </c>
-      <c r="F14" t="s">
-        <v>81</v>
-      </c>
-      <c r="G14" t="s">
-        <v>82</v>
-      </c>
-      <c r="H14" t="s">
-        <v>83</v>
-      </c>
-      <c r="I14" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="15">
@@ -1097,33 +1464,33 @@
         <v>2021</v>
       </c>
       <c r="B15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" t="s">
+        <v>84</v>
+      </c>
+      <c r="G15" t="s">
         <v>85</v>
       </c>
-      <c r="C15" t="s">
+      <c r="H15" t="s">
         <v>86</v>
       </c>
-      <c r="D15" t="s">
+      <c r="I15" t="s">
         <v>87</v>
-      </c>
-      <c r="E15" t="s">
-        <v>88</v>
-      </c>
-      <c r="F15" t="s">
-        <v>89</v>
-      </c>
-      <c r="G15" t="s">
-        <v>90</v>
-      </c>
-      <c r="H15" t="s">
-        <v>91</v>
-      </c>
-      <c r="I15" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18">
@@ -1131,16 +1498,16 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D18" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E18" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19">
@@ -1148,16 +1515,16 @@
         <v>2011</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C19" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E19" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20">
@@ -1165,16 +1532,16 @@
         <v>2012</v>
       </c>
       <c r="B20" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D20" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E20" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21">
@@ -1182,16 +1549,16 @@
         <v>2013</v>
       </c>
       <c r="B21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" t="s">
         <v>98</v>
       </c>
-      <c r="C21" t="s">
-        <v>103</v>
-      </c>
       <c r="D21" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E21" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22">
@@ -1199,16 +1566,16 @@
         <v>2014</v>
       </c>
       <c r="B22" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D22" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E22" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23">
@@ -1216,16 +1583,16 @@
         <v>2015</v>
       </c>
       <c r="B23" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C23" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D23" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E23" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24">
@@ -1233,16 +1600,16 @@
         <v>2016</v>
       </c>
       <c r="B24" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="C24" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="D24" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="E24" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25">
@@ -1250,16 +1617,16 @@
         <v>2017</v>
       </c>
       <c r="B25" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C25" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="D25" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="E25" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26">
@@ -1267,16 +1634,16 @@
         <v>2018</v>
       </c>
       <c r="B26" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C26" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="D26" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E26" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27">
@@ -1284,16 +1651,16 @@
         <v>2019</v>
       </c>
       <c r="B27" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="C27" t="s">
-        <v>125</v>
+        <v>93</v>
       </c>
       <c r="D27" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="E27" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28">
@@ -1301,16 +1668,16 @@
         <v>2020</v>
       </c>
       <c r="B28" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="C28" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
       <c r="D28" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E28" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29">
@@ -1318,16 +1685,629 @@
         <v>2021</v>
       </c>
       <c r="B29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" t="s">
+        <v>119</v>
+      </c>
+      <c r="D29" t="s">
+        <v>120</v>
+      </c>
+      <c r="E29" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="10.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="17.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="17.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="17.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="17.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="17.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="17.71" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="17.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="17.71" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="9.15" hidden="0" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" t="s">
+        <v>131</v>
+      </c>
+      <c r="I4" t="s">
         <v>132</v>
       </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5" t="s">
+        <v>133</v>
+      </c>
+      <c r="G5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H5" t="s">
+        <v>135</v>
+      </c>
+      <c r="I5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E6" t="s">
+        <v>140</v>
+      </c>
+      <c r="F6" t="s">
+        <v>141</v>
+      </c>
+      <c r="G6" t="s">
+        <v>142</v>
+      </c>
+      <c r="H6" t="s">
+        <v>143</v>
+      </c>
+      <c r="I6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G7" t="s">
+        <v>150</v>
+      </c>
+      <c r="H7" t="s">
+        <v>151</v>
+      </c>
+      <c r="I7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D8" t="s">
+        <v>155</v>
+      </c>
+      <c r="E8" t="s">
+        <v>156</v>
+      </c>
+      <c r="F8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G8" t="s">
+        <v>158</v>
+      </c>
+      <c r="H8" t="s">
+        <v>159</v>
+      </c>
+      <c r="I8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" t="s">
+        <v>162</v>
+      </c>
+      <c r="D9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E9" t="s">
+        <v>164</v>
+      </c>
+      <c r="F9" t="s">
+        <v>165</v>
+      </c>
+      <c r="G9" t="s">
+        <v>166</v>
+      </c>
+      <c r="H9" t="s">
+        <v>167</v>
+      </c>
+      <c r="I9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C10" t="s">
+        <v>170</v>
+      </c>
+      <c r="D10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E10" t="s">
+        <v>172</v>
+      </c>
+      <c r="F10" t="s">
+        <v>169</v>
+      </c>
+      <c r="G10" t="s">
+        <v>173</v>
+      </c>
+      <c r="H10" t="s">
+        <v>171</v>
+      </c>
+      <c r="I10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B11" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" t="s">
+        <v>176</v>
+      </c>
+      <c r="D11" t="s">
+        <v>177</v>
+      </c>
+      <c r="E11" t="s">
+        <v>178</v>
+      </c>
+      <c r="F11" t="s">
+        <v>179</v>
+      </c>
+      <c r="G11" t="s">
+        <v>180</v>
+      </c>
+      <c r="H11" t="s">
+        <v>181</v>
+      </c>
+      <c r="I11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B12" t="s">
+        <v>183</v>
+      </c>
+      <c r="C12" t="s">
+        <v>184</v>
+      </c>
+      <c r="D12" t="s">
+        <v>185</v>
+      </c>
+      <c r="E12" t="s">
+        <v>186</v>
+      </c>
+      <c r="F12" t="s">
+        <v>187</v>
+      </c>
+      <c r="G12" t="s">
+        <v>188</v>
+      </c>
+      <c r="H12" t="s">
+        <v>189</v>
+      </c>
+      <c r="I12" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B13" t="s">
+        <v>191</v>
+      </c>
+      <c r="C13" t="s">
+        <v>192</v>
+      </c>
+      <c r="D13" t="s">
+        <v>193</v>
+      </c>
+      <c r="E13" t="s">
+        <v>194</v>
+      </c>
+      <c r="F13" t="s">
+        <v>195</v>
+      </c>
+      <c r="G13" t="s">
+        <v>196</v>
+      </c>
+      <c r="H13" t="s">
+        <v>197</v>
+      </c>
+      <c r="I13" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B14" t="s">
+        <v>199</v>
+      </c>
+      <c r="C14" t="s">
+        <v>200</v>
+      </c>
+      <c r="D14" t="s">
+        <v>201</v>
+      </c>
+      <c r="E14" t="s">
+        <v>202</v>
+      </c>
+      <c r="F14" t="s">
+        <v>203</v>
+      </c>
+      <c r="G14" t="s">
+        <v>204</v>
+      </c>
+      <c r="H14" t="s">
+        <v>205</v>
+      </c>
+      <c r="I14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B15" t="s">
+        <v>207</v>
+      </c>
+      <c r="C15" t="s">
+        <v>208</v>
+      </c>
+      <c r="D15" t="s">
+        <v>209</v>
+      </c>
+      <c r="E15" t="s">
+        <v>210</v>
+      </c>
+      <c r="F15" t="s">
+        <v>211</v>
+      </c>
+      <c r="G15" t="s">
+        <v>212</v>
+      </c>
+      <c r="H15" t="s">
+        <v>213</v>
+      </c>
+      <c r="I15" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>215</v>
+      </c>
+      <c r="C18" t="s">
+        <v>216</v>
+      </c>
+      <c r="D18" t="s">
+        <v>217</v>
+      </c>
+      <c r="E18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B20" t="s">
+        <v>219</v>
+      </c>
+      <c r="C20" t="s">
+        <v>220</v>
+      </c>
+      <c r="D20" t="s">
+        <v>221</v>
+      </c>
+      <c r="E20" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B21" t="s">
+        <v>223</v>
+      </c>
+      <c r="C21" t="s">
+        <v>224</v>
+      </c>
+      <c r="D21" t="s">
+        <v>225</v>
+      </c>
+      <c r="E21" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B22" t="s">
+        <v>227</v>
+      </c>
+      <c r="C22" t="s">
+        <v>228</v>
+      </c>
+      <c r="D22" t="s">
+        <v>229</v>
+      </c>
+      <c r="E22" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B23" t="s">
+        <v>231</v>
+      </c>
+      <c r="C23" t="s">
+        <v>232</v>
+      </c>
+      <c r="D23" t="s">
+        <v>233</v>
+      </c>
+      <c r="E23" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" t="s">
+        <v>235</v>
+      </c>
+      <c r="D24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B25" t="s">
+        <v>237</v>
+      </c>
+      <c r="C25" t="s">
+        <v>238</v>
+      </c>
+      <c r="D25" t="s">
+        <v>239</v>
+      </c>
+      <c r="E25" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B26" t="s">
+        <v>241</v>
+      </c>
+      <c r="C26" t="s">
+        <v>242</v>
+      </c>
+      <c r="D26" t="s">
+        <v>243</v>
+      </c>
+      <c r="E26" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B27" t="s">
+        <v>245</v>
+      </c>
+      <c r="C27" t="s">
+        <v>246</v>
+      </c>
+      <c r="D27" t="s">
+        <v>247</v>
+      </c>
+      <c r="E27" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B28" t="s">
+        <v>249</v>
+      </c>
+      <c r="C28" t="s">
+        <v>250</v>
+      </c>
+      <c r="D28" t="s">
+        <v>251</v>
+      </c>
+      <c r="E28" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B29" t="s">
+        <v>253</v>
+      </c>
       <c r="C29" t="s">
-        <v>133</v>
+        <v>254</v>
       </c>
       <c r="D29" t="s">
-        <v>134</v>
+        <v>255</v>
       </c>
       <c r="E29" t="s">
-        <v>135</v>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>